<commit_message>
Creacion de script, para agregar eficiencia
</commit_message>
<xml_diff>
--- a/Modelo/graduados.xlsx
+++ b/Modelo/graduados.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="estudiantes_graduados" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -402,6 +402,11 @@
           <t>termino_egreso</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Eficiencia_Terminal</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -442,6 +447,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -481,6 +489,9 @@
         <is>
           <t>1S</t>
         </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -522,6 +533,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -562,6 +576,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -602,6 +619,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -642,6 +662,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -682,6 +705,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -722,6 +748,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -762,6 +791,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -802,6 +834,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -842,6 +877,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -882,6 +920,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -922,6 +963,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -962,6 +1006,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1002,6 +1049,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1042,6 +1092,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1082,6 +1135,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1122,6 +1178,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1162,6 +1221,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1202,6 +1264,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1242,6 +1307,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1282,6 +1350,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1322,6 +1393,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1362,6 +1436,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1402,6 +1479,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1442,6 +1522,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1482,6 +1565,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1522,6 +1608,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1562,6 +1651,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1602,6 +1694,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1642,6 +1737,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1682,6 +1780,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1722,6 +1823,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1762,6 +1866,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1802,6 +1909,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1842,6 +1952,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1882,6 +1995,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1922,6 +2038,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1962,6 +2081,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2002,6 +2124,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2042,6 +2167,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2082,6 +2210,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2122,6 +2253,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2162,6 +2296,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2202,6 +2339,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2242,6 +2382,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2282,6 +2425,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2322,6 +2468,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2362,6 +2511,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2402,6 +2554,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2442,6 +2597,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2482,6 +2640,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2522,6 +2683,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2562,6 +2726,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2602,6 +2769,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2642,6 +2812,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2682,6 +2855,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2722,6 +2898,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2762,6 +2941,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2802,6 +2984,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2842,6 +3027,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2882,6 +3070,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2922,6 +3113,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2962,6 +3156,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3002,6 +3199,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -3042,6 +3242,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3082,6 +3285,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3122,6 +3328,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3162,6 +3371,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -3202,6 +3414,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3242,6 +3457,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3282,6 +3500,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -3322,6 +3543,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3362,6 +3586,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -3402,6 +3629,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -3442,6 +3672,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -3482,6 +3715,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -3522,6 +3758,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -3562,6 +3801,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -3602,6 +3844,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -3642,6 +3887,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -3682,6 +3930,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -3722,6 +3973,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -3762,6 +4016,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3802,6 +4059,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3842,6 +4102,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -3882,6 +4145,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -3922,6 +4188,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -3962,6 +4231,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -4002,6 +4274,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -4042,6 +4317,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -4082,6 +4360,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -4122,6 +4403,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -4162,6 +4446,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -4202,6 +4489,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -4242,6 +4532,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -4282,6 +4575,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -4322,6 +4618,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I99" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -4362,6 +4661,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I100" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -4402,6 +4704,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -4442,6 +4747,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I102" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -4482,6 +4790,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -4522,6 +4833,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -4562,6 +4876,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -4602,6 +4919,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -4642,6 +4962,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -4682,6 +5005,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -4722,6 +5048,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -4762,6 +5091,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I110" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -4802,6 +5134,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -4842,6 +5177,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -4882,6 +5220,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -4922,6 +5263,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I114" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -4962,6 +5306,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -5002,6 +5349,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -5042,6 +5392,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -5082,6 +5435,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -5122,6 +5478,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I119" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -5162,6 +5521,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -5202,6 +5564,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -5242,6 +5607,9 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I122" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -5282,6 +5650,9 @@
           <t>2S</t>
         </is>
       </c>
+      <c r="I123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -5322,8 +5693,11 @@
           <t>1S</t>
         </is>
       </c>
+      <c r="I124" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>